<commit_message>
fixed gas dome problem
</commit_message>
<xml_diff>
--- a/02_Clean_data/5/CO2.xlsx
+++ b/02_Clean_data/5/CO2.xlsx
@@ -413,7 +413,7 @@
         <v>45140.54166666667</v>
       </c>
       <c r="B6">
-        <v>9670.300999999999</v>
+        <v>9670.301</v>
       </c>
     </row>
     <row r="7">
@@ -517,7 +517,7 @@
         <v>45141.08333333333</v>
       </c>
       <c r="B19">
-        <v>8378.543000000001</v>
+        <v>8378.543000000002</v>
       </c>
     </row>
     <row r="20">
@@ -541,7 +541,7 @@
         <v>45141.20833333333</v>
       </c>
       <c r="B22">
-        <v>8183.992999999999</v>
+        <v>8183.993</v>
       </c>
     </row>
     <row r="23">
@@ -733,7 +733,7 @@
         <v>45142.20833333333</v>
       </c>
       <c r="B46">
-        <v>7357.154</v>
+        <v>7357.154000000001</v>
       </c>
     </row>
     <row r="47">
@@ -741,7 +741,7 @@
         <v>45142.25</v>
       </c>
       <c r="B47">
-        <v>7364.306</v>
+        <v>7364.306000000001</v>
       </c>
     </row>
     <row r="48">
@@ -957,7 +957,7 @@
         <v>45143.375</v>
       </c>
       <c r="B74">
-        <v>7186.922</v>
+        <v>7186.922000000001</v>
       </c>
     </row>
     <row r="75">
@@ -1125,7 +1125,7 @@
         <v>45144.25</v>
       </c>
       <c r="B95">
-        <v>7278.474999999999</v>
+        <v>7278.475</v>
       </c>
     </row>
     <row r="96">
@@ -1277,7 +1277,7 @@
         <v>45145.04166666667</v>
       </c>
       <c r="B114">
-        <v>7357.154</v>
+        <v>7357.154000000001</v>
       </c>
     </row>
     <row r="115">
@@ -1461,7 +1461,7 @@
         <v>45146</v>
       </c>
       <c r="B137">
-        <v>7357.154</v>
+        <v>7357.154000000001</v>
       </c>
     </row>
     <row r="138">
@@ -1909,7 +1909,7 @@
         <v>45148.33333333333</v>
       </c>
       <c r="B193">
-        <v>6370.096</v>
+        <v>6370.096000000001</v>
       </c>
     </row>
     <row r="194">
@@ -1949,7 +1949,7 @@
         <v>45152.70833333333</v>
       </c>
       <c r="B198">
-        <v>4460.355</v>
+        <v>4460.355000000001</v>
       </c>
     </row>
     <row r="199">
@@ -2005,7 +2005,7 @@
         <v>45153</v>
       </c>
       <c r="B205">
-        <v>8713.284000000001</v>
+        <v>8713.284000000002</v>
       </c>
     </row>
     <row r="206">
@@ -2061,7 +2061,7 @@
         <v>45153.29166666667</v>
       </c>
       <c r="B212">
-        <v>8404.293000000001</v>
+        <v>8404.293000000002</v>
       </c>
     </row>
     <row r="213">
@@ -2157,7 +2157,7 @@
         <v>45153.79166666667</v>
       </c>
       <c r="B224">
-        <v>8836.309999999999</v>
+        <v>8836.31</v>
       </c>
     </row>
     <row r="225">
@@ -2373,7 +2373,7 @@
         <v>45154.91666666667</v>
       </c>
       <c r="B251">
-        <v>7983.721</v>
+        <v>7983.721000000001</v>
       </c>
     </row>
     <row r="252">
@@ -2389,7 +2389,7 @@
         <v>45155</v>
       </c>
       <c r="B253">
-        <v>7773.434999999999</v>
+        <v>7773.435</v>
       </c>
     </row>
     <row r="254">
@@ -2661,7 +2661,7 @@
         <v>45156.41666666667</v>
       </c>
       <c r="B287">
-        <v>7445.846</v>
+        <v>7445.846000000001</v>
       </c>
     </row>
     <row r="288">
@@ -2749,7 +2749,7 @@
         <v>45156.875</v>
       </c>
       <c r="B298">
-        <v>7377.181</v>
+        <v>7377.181000000001</v>
       </c>
     </row>
     <row r="299">
@@ -2773,7 +2773,7 @@
         <v>45157</v>
       </c>
       <c r="B301">
-        <v>7377.181</v>
+        <v>7377.181000000001</v>
       </c>
     </row>
     <row r="302">
@@ -2989,7 +2989,7 @@
         <v>45158.125</v>
       </c>
       <c r="B328">
-        <v>6943.733999999999</v>
+        <v>6943.734</v>
       </c>
     </row>
     <row r="329">
@@ -3061,7 +3061,7 @@
         <v>45158.5</v>
       </c>
       <c r="B337">
-        <v>6852.181</v>
+        <v>6852.181000000001</v>
       </c>
     </row>
     <row r="338">
@@ -3357,7 +3357,7 @@
         <v>45160.04166666667</v>
       </c>
       <c r="B374">
-        <v>6471.663</v>
+        <v>6471.663000000001</v>
       </c>
     </row>
     <row r="375">
@@ -3645,7 +3645,7 @@
         <v>45169.25</v>
       </c>
       <c r="B410">
-        <v>8057.992999999999</v>
+        <v>8057.993</v>
       </c>
     </row>
     <row r="411">
@@ -3845,7 +3845,7 @@
         <v>45170.29166666667</v>
       </c>
       <c r="B435">
-        <v>7444.681</v>
+        <v>7444.681000000001</v>
       </c>
     </row>
     <row r="436">
@@ -4525,7 +4525,7 @@
         <v>45173.83333333333</v>
       </c>
       <c r="B520">
-        <v>6560.355</v>
+        <v>6560.355000000001</v>
       </c>
     </row>
     <row r="521">
@@ -4613,7 +4613,7 @@
         <v>45174.29166666667</v>
       </c>
       <c r="B531">
-        <v>6373.733999999999</v>
+        <v>6373.734</v>
       </c>
     </row>
     <row r="532">
@@ -4669,7 +4669,7 @@
         <v>45174.58333333333</v>
       </c>
       <c r="B538">
-        <v>6228.474999999999</v>
+        <v>6228.475</v>
       </c>
     </row>
     <row r="539">
@@ -4693,7 +4693,7 @@
         <v>45174.70833333333</v>
       </c>
       <c r="B541">
-        <v>6111.172</v>
+        <v>6111.172000000001</v>
       </c>
     </row>
     <row r="542">
@@ -4741,7 +4741,7 @@
         <v>45174.95833333333</v>
       </c>
       <c r="B547">
-        <v>6176.376999999999</v>
+        <v>6176.377</v>
       </c>
     </row>
     <row r="548">
@@ -6925,7 +6925,7 @@
         <v>45149.33333333333</v>
       </c>
       <c r="B820">
-        <v>4494.279</v>
+        <v>4494.279000000001</v>
       </c>
     </row>
     <row r="821">
@@ -9445,7 +9445,7 @@
         <v>45162.45833333333</v>
       </c>
       <c r="B1135">
-        <v>4618.529</v>
+        <v>4618.529000000001</v>
       </c>
     </row>
     <row r="1136">
@@ -9629,7 +9629,7 @@
         <v>45163.41666666667</v>
       </c>
       <c r="B1158">
-        <v>4494.279</v>
+        <v>4494.279000000001</v>
       </c>
     </row>
     <row r="1159">
@@ -9909,7 +9909,7 @@
         <v>45164.875</v>
       </c>
       <c r="B1193">
-        <v>4494.279</v>
+        <v>4494.279000000001</v>
       </c>
     </row>
     <row r="1194">
@@ -13941,7 +13941,7 @@
         <v>45185.875</v>
       </c>
       <c r="B1697">
-        <v>4273.904</v>
+        <v>4273.904000000001</v>
       </c>
     </row>
     <row r="1698">
@@ -14173,7 +14173,7 @@
         <v>45187.08333333333</v>
       </c>
       <c r="B1726">
-        <v>4136.029</v>
+        <v>4136.029000000001</v>
       </c>
     </row>
     <row r="1727">
@@ -15245,7 +15245,7 @@
         <v>45192.66666666667</v>
       </c>
       <c r="B1860">
-        <v>4406.404</v>
+        <v>4406.404000000001</v>
       </c>
     </row>
     <row r="1861">
@@ -16053,7 +16053,7 @@
         <v>45196.875</v>
       </c>
       <c r="B1961">
-        <v>4136.029</v>
+        <v>4136.029000000001</v>
       </c>
     </row>
     <row r="1962">
@@ -17925,7 +17925,7 @@
         <v>45149.33333333333</v>
       </c>
       <c r="B2195">
-        <v>4494.279</v>
+        <v>4494.279000000001</v>
       </c>
     </row>
     <row r="2196">
@@ -20445,7 +20445,7 @@
         <v>45162.45833333333</v>
       </c>
       <c r="B2510">
-        <v>4618.529</v>
+        <v>4618.529000000001</v>
       </c>
     </row>
     <row r="2511">
@@ -20629,7 +20629,7 @@
         <v>45163.41666666667</v>
       </c>
       <c r="B2533">
-        <v>4494.279</v>
+        <v>4494.279000000001</v>
       </c>
     </row>
     <row r="2534">
@@ -20909,7 +20909,7 @@
         <v>45164.875</v>
       </c>
       <c r="B2568">
-        <v>4494.279</v>
+        <v>4494.279000000001</v>
       </c>
     </row>
     <row r="2569">
@@ -24941,7 +24941,7 @@
         <v>45185.875</v>
       </c>
       <c r="B3072">
-        <v>4273.904</v>
+        <v>4273.904000000001</v>
       </c>
     </row>
     <row r="3073">
@@ -25173,7 +25173,7 @@
         <v>45187.08333333333</v>
       </c>
       <c r="B3101">
-        <v>4136.029</v>
+        <v>4136.029000000001</v>
       </c>
     </row>
     <row r="3102">
@@ -26245,7 +26245,7 @@
         <v>45192.66666666667</v>
       </c>
       <c r="B3235">
-        <v>4406.404</v>
+        <v>4406.404000000001</v>
       </c>
     </row>
     <row r="3236">
@@ -27053,7 +27053,7 @@
         <v>45196.875</v>
       </c>
       <c r="B3336">
-        <v>4136.029</v>
+        <v>4136.029000000001</v>
       </c>
     </row>
     <row r="3337">
@@ -27773,7 +27773,7 @@
         <v>45200.625</v>
       </c>
       <c r="B3426">
-        <v>4132.404</v>
+        <v>4132.404000000001</v>
       </c>
     </row>
     <row r="3427">
@@ -32573,7 +32573,7 @@
         <v>45149.33333333333</v>
       </c>
       <c r="B4026">
-        <v>4494.279</v>
+        <v>4494.279000000001</v>
       </c>
     </row>
     <row r="4027">
@@ -35093,7 +35093,7 @@
         <v>45162.45833333333</v>
       </c>
       <c r="B4341">
-        <v>4618.529</v>
+        <v>4618.529000000001</v>
       </c>
     </row>
     <row r="4342">
@@ -35277,7 +35277,7 @@
         <v>45163.41666666667</v>
       </c>
       <c r="B4364">
-        <v>4494.279</v>
+        <v>4494.279000000001</v>
       </c>
     </row>
     <row r="4365">
@@ -35557,7 +35557,7 @@
         <v>45164.875</v>
       </c>
       <c r="B4399">
-        <v>4494.279</v>
+        <v>4494.279000000001</v>
       </c>
     </row>
     <row r="4400">
@@ -39589,7 +39589,7 @@
         <v>45185.875</v>
       </c>
       <c r="B4903">
-        <v>4273.904</v>
+        <v>4273.904000000001</v>
       </c>
     </row>
     <row r="4904">
@@ -39821,7 +39821,7 @@
         <v>45187.08333333333</v>
       </c>
       <c r="B4932">
-        <v>4136.029</v>
+        <v>4136.029000000001</v>
       </c>
     </row>
     <row r="4933">
@@ -40893,7 +40893,7 @@
         <v>45192.66666666667</v>
       </c>
       <c r="B5066">
-        <v>4406.404</v>
+        <v>4406.404000000001</v>
       </c>
     </row>
     <row r="5067">
@@ -41701,7 +41701,7 @@
         <v>45196.875</v>
       </c>
       <c r="B5167">
-        <v>4136.029</v>
+        <v>4136.029000000001</v>
       </c>
     </row>
     <row r="5168">
@@ -42421,7 +42421,7 @@
         <v>45200.625</v>
       </c>
       <c r="B5257">
-        <v>4132.404</v>
+        <v>4132.404000000001</v>
       </c>
     </row>
     <row r="5258">

</xml_diff>